<commit_message>
Form Certificate and Electrical Permit
</commit_message>
<xml_diff>
--- a/Documentation/LogSheet.xlsx
+++ b/Documentation/LogSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\BPA-NMH\OtherResources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\BPA-NMH\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EC5F14-226F-4DF6-9301-5A1A6F96FD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02566F0A-1744-4B2B-A553-91D6DFAB313C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41AD1B7F-CBDD-4F7F-BDC8-BE4B0735AB1A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>TASKS</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>In-progress</t>
+  </si>
+  <si>
+    <t>06/21/2023</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Design Presentation</t>
   </si>
 </sst>
 </file>
@@ -469,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22285EA-6BF3-4579-B0D4-962A2153141D}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,9 +588,105 @@
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>